<commit_message>
Updated test cases, log file,HomePage, UsedCarPage
</commit_message>
<xml_diff>
--- a/test-output/PopularCarModels.xlsx
+++ b/test-output/PopularCarModels.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="9">
   <si>
     <t>Popular Car Name</t>
   </si>
@@ -83,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A81"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -134,6 +134,366 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Last and the Final Code
</commit_message>
<xml_diff>
--- a/test-output/PopularCarModels.xlsx
+++ b/test-output/PopularCarModels.xlsx
@@ -12,33 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="2">
   <si>
     <t>Popular Car Name</t>
   </si>
   <si>
-    <t>Maruti 800</t>
-  </si>
-  <si>
-    <t>Maruti Swift</t>
-  </si>
-  <si>
-    <t>Hyundai I10</t>
-  </si>
-  <si>
-    <t>Hyundai Santro Xing</t>
-  </si>
-  <si>
-    <t>Honda City</t>
-  </si>
-  <si>
-    <t>Toyota Innova</t>
-  </si>
-  <si>
-    <t>Toyota Fortuner</t>
-  </si>
-  <si>
-    <t>Mahindra XUV500</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -101,37 +80,37 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>